<commit_message>
Add test points and pads
</commit_message>
<xml_diff>
--- a/electrical_design/LED_resistors.xlsx
+++ b/electrical_design/LED_resistors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/aagrahar_uwaterloo_ca/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tron\4B\MTE 482\Interface-PCB\electrical_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DFE7A8D-8894-44B6-AECC-D041326F8EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25581464-C6D4-4D42-980D-8EBBF2C60DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5415" yWindow="1770" windowWidth="28800" windowHeight="15555" xr2:uid="{0DB087E7-7223-437B-8069-21B1D5F0AC0C}"/>
+    <workbookView xWindow="16260" yWindow="1365" windowWidth="28800" windowHeight="15555" xr2:uid="{0DB087E7-7223-437B-8069-21B1D5F0AC0C}"/>
   </bookViews>
   <sheets>
     <sheet name="LED Resistor Calc" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>SMD</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Purpose</t>
+  </si>
+  <si>
+    <t>YELLOW</t>
   </si>
 </sst>
 </file>
@@ -187,15 +190,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,7 +639,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -647,14 +650,14 @@
   <dimension ref="B3:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
@@ -664,52 +667,52 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4">
         <v>12</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>2</v>
       </c>
       <c r="F4" s="4">
         <v>1.85</v>
@@ -737,18 +740,18 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="4">
         <v>12</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F5" s="4">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="G5" s="4">
         <v>20</v>
@@ -758,32 +761,32 @@
       </c>
       <c r="I5" s="3">
         <f>(C5-F5)/(H5*10^-3)</f>
-        <v>660</v>
+        <v>680</v>
       </c>
       <c r="J5" s="1">
         <v>680</v>
       </c>
       <c r="K5" s="2">
         <f>(C5-F5)/J5*10^3</f>
-        <v>14.558823529411764</v>
+        <v>15</v>
       </c>
       <c r="L5" s="1">
         <f>(C5-F5)*K5*10^-3</f>
-        <v>0.14413235294117646</v>
+        <v>0.153</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4">
         <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>2</v>
       </c>
       <c r="F6" s="4">
         <v>2.1</v>
@@ -799,30 +802,30 @@
         <v>193.33333333333334</v>
       </c>
       <c r="J6" s="1">
-        <v>200</v>
+        <v>220</v>
       </c>
       <c r="K6" s="2">
         <f>(C6-F6)/J6*10^3</f>
-        <v>14.499999999999998</v>
+        <v>13.181818181818182</v>
       </c>
       <c r="L6" s="1">
         <f>(C6-F6)*K6*10^-3</f>
-        <v>4.204999999999999E-2</v>
+        <v>3.8227272727272728E-2</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
+      <c r="B7" s="8"/>
       <c r="C7" s="4">
         <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>0</v>
-      </c>
       <c r="F7" s="4">
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="G7" s="4">
         <v>20</v>
@@ -832,32 +835,32 @@
       </c>
       <c r="I7" s="3">
         <f>(C7-F7)/(H7*10^-3)</f>
-        <v>133.33333333333334</v>
+        <v>173.33333333333334</v>
       </c>
       <c r="J7" s="1">
-        <v>130</v>
+        <v>220</v>
       </c>
       <c r="K7" s="2">
         <f>(C7-F7)/J7*10^3</f>
-        <v>15.384615384615385</v>
+        <v>11.818181818181818</v>
       </c>
       <c r="L7" s="1">
         <f>(C7-F7)*K7*10^-3</f>
-        <v>3.0769230769230771E-2</v>
+        <v>3.0727272727272732E-2</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="4">
         <v>3.3</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>2</v>
       </c>
       <c r="F8" s="4">
         <v>1.85</v>
@@ -885,15 +888,15 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
+      <c r="B9" s="8"/>
       <c r="C9" s="4">
         <v>3.3</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>0</v>
       </c>
       <c r="F9" s="4">
         <v>3</v>
@@ -909,15 +912,15 @@
         <v>19.999999999999989</v>
       </c>
       <c r="J9" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K9" s="2">
         <f>(C9-F9)/J9*10^3</f>
-        <v>14.999999999999991</v>
+        <v>13.63636363636363</v>
       </c>
       <c r="L9" s="1">
         <f>(C9-F9)*K9*10^-3</f>
-        <v>4.4999999999999945E-3</v>
+        <v>4.0909090909090869E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Blue LED resistor value
</commit_message>
<xml_diff>
--- a/electrical_design/LED_resistors.xlsx
+++ b/electrical_design/LED_resistors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tron\4B\MTE 482\Interface-PCB\electrical_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25581464-C6D4-4D42-980D-8EBBF2C60DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38AAFE75-B147-4143-8315-AF1A9EB1B590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16260" yWindow="1365" windowWidth="28800" windowHeight="15555" xr2:uid="{0DB087E7-7223-437B-8069-21B1D5F0AC0C}"/>
+    <workbookView xWindow="4065" yWindow="5595" windowWidth="28800" windowHeight="15555" xr2:uid="{0DB087E7-7223-437B-8069-21B1D5F0AC0C}"/>
   </bookViews>
   <sheets>
     <sheet name="LED Resistor Calc" sheetId="1" r:id="rId1"/>
@@ -650,7 +650,7 @@
   <dimension ref="B3:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,18 +724,18 @@
         <v>15</v>
       </c>
       <c r="I4" s="3">
-        <f>(C4-F4)/(H4*10^-3)</f>
+        <f t="shared" ref="I4:I9" si="0">(C4-F4)/(H4*10^-3)</f>
         <v>676.66666666666674</v>
       </c>
       <c r="J4" s="1">
         <v>680</v>
       </c>
       <c r="K4" s="2">
-        <f>(C4-F4)/J4*10^3</f>
+        <f t="shared" ref="K4:K9" si="1">(C4-F4)/J4*10^3</f>
         <v>14.926470588235295</v>
       </c>
       <c r="L4" s="1">
-        <f>(C4-F4)*K4*10^-3</f>
+        <f t="shared" ref="L4:L9" si="2">(C4-F4)*K4*10^-3</f>
         <v>0.15150367647058827</v>
       </c>
     </row>
@@ -760,18 +760,18 @@
         <v>15</v>
       </c>
       <c r="I5" s="3">
-        <f>(C5-F5)/(H5*10^-3)</f>
+        <f t="shared" si="0"/>
         <v>680</v>
       </c>
       <c r="J5" s="1">
         <v>680</v>
       </c>
       <c r="K5" s="2">
-        <f>(C5-F5)/J5*10^3</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="L5" s="1">
-        <f>(C5-F5)*K5*10^-3</f>
+        <f t="shared" si="2"/>
         <v>0.153</v>
       </c>
     </row>
@@ -798,18 +798,18 @@
         <v>15</v>
       </c>
       <c r="I6" s="3">
-        <f>(C6-F6)/(H6*10^-3)</f>
+        <f t="shared" si="0"/>
         <v>193.33333333333334</v>
       </c>
       <c r="J6" s="1">
         <v>220</v>
       </c>
       <c r="K6" s="2">
-        <f>(C6-F6)/J6*10^3</f>
+        <f t="shared" si="1"/>
         <v>13.181818181818182</v>
       </c>
       <c r="L6" s="1">
-        <f>(C6-F6)*K6*10^-3</f>
+        <f t="shared" si="2"/>
         <v>3.8227272727272728E-2</v>
       </c>
     </row>
@@ -834,18 +834,18 @@
         <v>15</v>
       </c>
       <c r="I7" s="3">
-        <f>(C7-F7)/(H7*10^-3)</f>
+        <f t="shared" si="0"/>
         <v>173.33333333333334</v>
       </c>
       <c r="J7" s="1">
         <v>220</v>
       </c>
       <c r="K7" s="2">
-        <f>(C7-F7)/J7*10^3</f>
+        <f t="shared" si="1"/>
         <v>11.818181818181818</v>
       </c>
       <c r="L7" s="1">
-        <f>(C7-F7)*K7*10^-3</f>
+        <f t="shared" si="2"/>
         <v>3.0727272727272732E-2</v>
       </c>
     </row>
@@ -872,18 +872,18 @@
         <v>15</v>
       </c>
       <c r="I8" s="3">
-        <f>(C8-F8)/(H8*10^-3)</f>
+        <f t="shared" si="0"/>
         <v>96.666666666666657</v>
       </c>
       <c r="J8" s="1">
         <v>100</v>
       </c>
       <c r="K8" s="2">
-        <f>(C8-F8)/J8*10^3</f>
+        <f t="shared" si="1"/>
         <v>14.499999999999996</v>
       </c>
       <c r="L8" s="1">
-        <f>(C8-F8)*K8*10^-3</f>
+        <f t="shared" si="2"/>
         <v>2.1024999999999992E-2</v>
       </c>
     </row>
@@ -908,18 +908,18 @@
         <v>15</v>
       </c>
       <c r="I9" s="3">
-        <f>(C9-F9)/(H9*10^-3)</f>
+        <f t="shared" si="0"/>
         <v>19.999999999999989</v>
       </c>
       <c r="J9" s="1">
         <v>22</v>
       </c>
       <c r="K9" s="2">
-        <f>(C9-F9)/J9*10^3</f>
+        <f t="shared" si="1"/>
         <v>13.63636363636363</v>
       </c>
       <c r="L9" s="1">
-        <f>(C9-F9)*K9*10^-3</f>
+        <f t="shared" si="2"/>
         <v>4.0909090909090869E-3</v>
       </c>
     </row>

</xml_diff>